<commit_message>
changed constraint about landing dist corvo
</commit_message>
<xml_diff>
--- a/Azores_Flight_Data_v3.xlsx
+++ b/Azores_Flight_Data_v3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils de Krom\Desktop\Operations Optimisation Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils de Krom\Documents\GitHub\Operations_optimization_assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80B27D0-2BA8-4385-AAC0-B13F1FF54C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3855E452-5406-494F-B083-EF0AE93B38A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand Table" sheetId="4" r:id="rId1"/>
@@ -4185,7 +4185,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Continued looking at demand and pickup
</commit_message>
<xml_diff>
--- a/Azores_Flight_Data_v3.xlsx
+++ b/Azores_Flight_Data_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils de Krom\Documents\GitHub\Operations_optimization_assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3855E452-5406-494F-B083-EF0AE93B38A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250A8612-CE29-4CF5-A3A8-DBE2D25C3251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4185,7 +4185,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>